<commit_message>
[zvnl 4400] quickdrive scenario
</commit_message>
<xml_diff>
--- a/zvnl-2022.xlsx
+++ b/zvnl-2022.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062CD99B-1F26-42C4-992C-6FEE9E311608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8E9C13-B69F-4DCC-8B4B-13A9191E389C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1980" windowWidth="21503" windowHeight="12975" activeTab="2" xr2:uid="{9EB046AB-1F2A-445C-8D11-2727B0F917E9}"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="21503" windowHeight="12975" activeTab="3" xr2:uid="{9EB046AB-1F2A-445C-8D11-2727B0F917E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Spotten" sheetId="2" r:id="rId1"/>
     <sheet name="Standard" sheetId="1" r:id="rId2"/>
     <sheet name="QD consists" sheetId="3" r:id="rId3"/>
-    <sheet name="QD Goederen" sheetId="4" r:id="rId4"/>
-    <sheet name="QD" sheetId="5" r:id="rId5"/>
+    <sheet name="QD" sheetId="5" r:id="rId4"/>
+    <sheet name="QD Goederen" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'QD consists'!$A$1:$G$30</definedName>
@@ -76,6 +76,40 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{F2EC6619-21D8-469B-8F2E-ADA1236E0886}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Grupo_STR, Kuju, RSItalia?, DTG KS en TGV, Rubku_NL/Decals</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -381,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
   <si>
     <t>Naam</t>
   </si>
@@ -775,13 +809,76 @@
     <t>ARR GTW-D 2/6</t>
   </si>
   <si>
-    <t>Rubku_NL/Decals</t>
-  </si>
-  <si>
-    <t>Kuju/RailSimulator</t>
-  </si>
-  <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Jaartal</t>
+  </si>
+  <si>
+    <t>Standaard includes</t>
+  </si>
+  <si>
+    <t>4400 Ehv-Ht</t>
+  </si>
+  <si>
+    <t>- Ehv
+- Btl</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>- 800 Ehv-Bet</t>
+  </si>
+  <si>
+    <t>Ehv:
+- 3900 Ehv2</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Ehv-Ht:
+- 6400 Ehs
+- G Ehs
+- 3500 At
+- 1100 At
+- G 2x Bet
+- 4400 Bet
+- 800 Beto
+- 1900 Beto
+- G Beto-Lpe
+- G Lpe
+- 6400 Btl
+- 3900 Btl
+- G Btl-Vg
+- 3500 Vga
+- 4400 Vga</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>Ht:
+- 800 Ht6
+- 6000 Ht4a
+- 6600 Ht7</t>
+  </si>
+  <si>
+    <t>- At
+- Ht</t>
   </si>
 </sst>
 </file>
@@ -894,7 +991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -925,6 +1022,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1483,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99201481-4895-4823-A291-1CA364EA89DE}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1538,141 +1640,150 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="10">
-        <v>3600</v>
+        <v>1900</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
-        <v>33</v>
+      <c r="A4" s="10">
+        <v>2000</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="10">
-        <v>7200</v>
+        <v>2800</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
-        <v>59</v>
+      <c r="A6" s="10">
+        <v>3000</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
-        <v>37</v>
+      <c r="A7" s="10">
+        <v>3100</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
-        <v>5700</v>
+        <v>3200</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
-        <v>34</v>
+      <c r="A9" s="10">
+        <v>3600</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="10">
-        <v>5500</v>
+        <v>3900</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>41</v>
@@ -1681,29 +1792,35 @@
         <v>44</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="10">
-        <v>6000</v>
+        <v>4400</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
-        <v>6900</v>
+        <v>5500</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>53</v>
@@ -1717,44 +1834,50 @@
       <c r="E12" s="18" t="s">
         <v>62</v>
       </c>
+      <c r="F12" s="9" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="10">
-        <v>7300</v>
+        <v>5600</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
-        <v>7400</v>
+        <v>5700</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="10">
-        <v>8900</v>
+        <v>6000</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>53</v>
@@ -1768,47 +1891,56 @@
       <c r="E15" s="18" t="s">
         <v>62</v>
       </c>
+      <c r="F15" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="10">
-        <v>3000</v>
+        <v>6400</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="10">
-        <v>3100</v>
+        <v>6600</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
-        <v>3200</v>
+        <v>6900</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>41</v>
@@ -1817,32 +1949,35 @@
         <v>44</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="10">
-        <v>3900</v>
+        <v>7200</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>31</v>
+      <c r="A20" s="10">
+        <v>7300</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>41</v>
@@ -1851,202 +1986,214 @@
         <v>44</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
-        <v>30</v>
+      <c r="A21" s="10">
+        <v>7400</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="10">
-        <v>1900</v>
+        <v>8900</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="10">
-        <v>2000</v>
+        <v>28300</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="10">
-        <v>2800</v>
+      <c r="A24" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="10">
-        <v>5600</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="E27" s="18" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="10">
-        <v>28300</v>
+      <c r="A28" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="10">
-        <v>4400</v>
+      <c r="A29" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="10">
-        <v>6400</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>65</v>
+      <c r="A30" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="19">
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="10">
-        <v>6600</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>65</v>
+      <c r="A31" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="19">
+        <v>9.0000000000000011E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
         <v>99</v>
@@ -2060,120 +2207,126 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G33" s="19">
-        <v>0.04</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G34" s="19">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G35" s="19">
-        <v>0.02</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G36" s="19">
-        <v>5.0000000000000002E-5</v>
+        <v>6.0000000000000005E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G37" s="19">
-        <v>6.0000000000000005E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G38" s="19">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" t="s">
-        <v>97</v>
-      </c>
-      <c r="G39" s="19">
-        <v>0.33</v>
+        <v>36</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" t="s">
-        <v>98</v>
-      </c>
-      <c r="G40" s="19">
-        <v>9.0000000000000011E-2</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G30" xr:uid="{99201481-4895-4823-A291-1CA364EA89DE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
-      <sortCondition ref="E1:E30"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
+      <sortCondition ref="A1:A30"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2182,11 +2335,132 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625C668E-F158-47C3-92FC-73333CE40EFC}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="7">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="1"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4016841F-3F20-4E64-B07C-6A68DCF27BDB}">
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F31"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2646,29 +2920,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625C668E-F158-47C3-92FC-73333CE40EFC}">
-  <dimension ref="E19:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[zvnl 6400] scenario Ehv-Tbu
</commit_message>
<xml_diff>
--- a/zvnl-2022.xlsx
+++ b/zvnl-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8E9C13-B69F-4DCC-8B4B-13A9191E389C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F20470-9623-498E-977A-15B672B95299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1380" windowWidth="21503" windowHeight="12975" activeTab="3" xr2:uid="{9EB046AB-1F2A-445C-8D11-2727B0F917E9}"/>
   </bookViews>
@@ -415,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="138">
   <si>
     <t>Naam</t>
   </si>
@@ -850,7 +850,37 @@
     <t>90</t>
   </si>
   <si>
-    <t>Ehv-Ht:
+    <t>180</t>
+  </si>
+  <si>
+    <t>Ht:
+- 800 Ht6
+- 6000 Ht4a
+- 6600 Ht7</t>
+  </si>
+  <si>
+    <t>- At
+- Ht</t>
+  </si>
+  <si>
+    <t>6400 Ehv-Tb</t>
+  </si>
+  <si>
+    <t>- Ehv</t>
+  </si>
+  <si>
+    <t>Ehv:
+- geen</t>
+  </si>
+  <si>
+    <t>Btl-Ht:
+- 3900 Btl
+- G Btl-Vg
+- 3500 Vga
+- 4400 Vga</t>
+  </si>
+  <si>
+    <t>Ehv-Btl:
 - 6400 Ehs
 - G Ehs
 - 3500 At
@@ -861,24 +891,34 @@
 - 1900 Beto
 - G Beto-Lpe
 - G Lpe
-- 6400 Btl
-- 3900 Btl
-- G Btl-Vg
-- 3500 Vga
-- 4400 Vga</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>Ht:
-- 800 Ht6
-- 6000 Ht4a
-- 6600 Ht7</t>
-  </si>
-  <si>
-    <t>- At
-- Ht</t>
+- 6400 Btl</t>
+  </si>
+  <si>
+    <t>Ehb-Btl:
+- 800 Ehs
+- 4400 Ehs
+- G 2x At
+- 3900 Bet
+- 6400 Bet
+- G 2x Beto
+- 3500 Lpe
+- 1100 Lpe
+- 4400 Btl</t>
+  </si>
+  <si>
+    <t>Btl-Tbu:
+- G Btl-Otw
+- 6400 Otw
+- G Otw-Tba
+- 1100 Tb
+- G Tbu</t>
+  </si>
+  <si>
+    <t>- G voor sp
+- 3900 achter sp</t>
+  </si>
+  <si>
+    <t>- At</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1626,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1892,7 +1932,7 @@
         <v>62</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -2009,7 +2049,7 @@
         <v>62</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -2029,7 +2069,7 @@
         <v>62</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -2336,115 +2376,155 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625C668E-F158-47C3-92FC-73333CE40EFC}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="7">
         <v>3022</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C2" s="7">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="228" x14ac:dyDescent="0.45">
+      <c r="C4" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="171" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>